<commit_message>
Add to BOM parts for "internal" Teensy pins
These are needed for driving valves 33-51.
</commit_message>
<xml_diff>
--- a/HMS Olfactometer v2 BOM.xlsx
+++ b/HMS Olfactometer v2 BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="55480" yWindow="940" windowWidth="27860" windowHeight="21440" tabRatio="500"/>
+    <workbookView xWindow="20800" yWindow="880" windowWidth="27860" windowHeight="23020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
   <si>
     <t>Vendor</t>
   </si>
@@ -87,9 +87,6 @@
     <t>8-way NPN</t>
   </si>
   <si>
-    <t>Connectors</t>
-  </si>
-  <si>
     <t>BNC</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>Passives</t>
   </si>
   <si>
-    <t>We have them</t>
-  </si>
-  <si>
     <t>PJRC</t>
   </si>
   <si>
@@ -198,9 +192,6 @@
     <t>S7041-ND</t>
   </si>
   <si>
-    <t>Only when using all 51 valves</t>
-  </si>
-  <si>
     <t>ED1515-ND</t>
   </si>
   <si>
@@ -225,9 +216,6 @@
     <t>C11:  4.7µF  50V,  1812</t>
   </si>
   <si>
-    <t>C1:  7µF  50V,  1812</t>
-  </si>
-  <si>
     <t>We have these in shop</t>
   </si>
   <si>
@@ -256,6 +244,54 @@
   </si>
   <si>
     <t xml:space="preserve"> 490-12457-1-ND</t>
+  </si>
+  <si>
+    <t>Minimum order of 3 to qualify for the $33 special</t>
+  </si>
+  <si>
+    <t>609-5751-ND</t>
+  </si>
+  <si>
+    <t>609-5752-ND</t>
+  </si>
+  <si>
+    <t>S7106-ND</t>
+  </si>
+  <si>
+    <t>S7107-ND</t>
+  </si>
+  <si>
+    <t>2x3-pin header (central pins)</t>
+  </si>
+  <si>
+    <t>2x4-pin header (central pins)</t>
+  </si>
+  <si>
+    <t>2x3-pin socket (central pins)</t>
+  </si>
+  <si>
+    <t>2x4-pin socket (central pins)</t>
+  </si>
+  <si>
+    <t>24-pin header (sides)</t>
+  </si>
+  <si>
+    <t>3M155862-24-ND</t>
+  </si>
+  <si>
+    <t>Connectors for 32 channel version</t>
+  </si>
+  <si>
+    <t>Additional connectors for channels 33-51</t>
+  </si>
+  <si>
+    <t>Not all 7 are needed, depending on how many valves you use</t>
+  </si>
+  <si>
+    <t>Only needed if you order the Teensy 3.5 without pins</t>
+  </si>
+  <si>
+    <t>C1:  6.8µF  50V,  1812</t>
   </si>
 </sst>
 </file>
@@ -339,7 +375,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -377,8 +413,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -389,8 +431,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -409,6 +454,9 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -427,6 +475,9 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -759,11 +810,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:I58"/>
+  <dimension ref="B2:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
+      <pane ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -777,7 +828,7 @@
   <sheetData>
     <row r="2" spans="2:9" ht="25">
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:9" s="2" customFormat="1">
@@ -872,7 +923,7 @@
         <v>849.12</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:9">
@@ -883,7 +934,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E10">
         <v>6</v>
@@ -896,18 +947,18 @@
         <v>612.06000000000006</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:9">
       <c r="B11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -917,18 +968,18 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -955,7 +1006,7 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -967,25 +1018,16 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="2:9">
-      <c r="G16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="G17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
+      <c r="I15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
       <c r="B18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -998,30 +1040,20 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
-      <c r="G19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:9">
       <c r="B20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
+    </row>
+    <row r="21" spans="2:9">
       <c r="B21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1034,9 +1066,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:9">
       <c r="B22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1045,15 +1077,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:9">
       <c r="B23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1066,15 +1098,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:9">
       <c r="B24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1087,36 +1119,20 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
-      <c r="G25" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="G26" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="2:9">
       <c r="B27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7">
+    </row>
+    <row r="28" spans="2:9">
       <c r="B28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1129,22 +1145,12 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="29" spans="2:7">
-      <c r="G29" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7">
+    <row r="30" spans="2:9">
       <c r="B30" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7">
+    </row>
+    <row r="31" spans="2:9">
       <c r="B31" t="s">
         <v>21</v>
       </c>
@@ -1152,7 +1158,7 @@
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E31">
         <v>7</v>
@@ -1164,31 +1170,24 @@
         <f t="shared" si="0"/>
         <v>9.1</v>
       </c>
-    </row>
-    <row r="32" spans="2:7">
-      <c r="G32" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="I31" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="2:9">
       <c r="B33" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="18">
       <c r="B34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E34">
         <v>2</v>
@@ -1203,13 +1202,13 @@
     </row>
     <row r="35" spans="2:9" ht="18">
       <c r="B35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1224,13 +1223,13 @@
     </row>
     <row r="36" spans="2:9">
       <c r="B36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -1242,13 +1241,13 @@
     </row>
     <row r="37" spans="2:9">
       <c r="B37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -1260,260 +1259,371 @@
     </row>
     <row r="38" spans="2:9">
       <c r="B38" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38">
+      <c r="E38" s="10">
         <v>8</v>
       </c>
       <c r="F38" s="3">
         <v>1.43</v>
       </c>
       <c r="G38" s="3">
-        <f t="shared" ref="G38:G52" si="1">E38*F38</f>
+        <f t="shared" ref="G38:G60" si="1">E38*F38</f>
         <v>11.44</v>
       </c>
       <c r="I38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="6"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="39" spans="2:9">
-      <c r="B39" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" t="s">
-        <v>58</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39" s="3">
+      <c r="E41" s="10">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3">
         <v>0.67</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G41" s="3">
+        <f>E41*F41</f>
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="10">
+        <v>2</v>
+      </c>
+      <c r="F42" s="3">
+        <v>1.43</v>
+      </c>
+      <c r="G42" s="3">
+        <f t="shared" ref="G42:G47" si="2">E42*F42</f>
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="12">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="G43" s="3">
+        <f t="shared" si="2"/>
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" s="12">
+        <v>2</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="G44" s="3">
+        <f t="shared" si="2"/>
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="B45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" s="12">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G45" s="3">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9">
+      <c r="B46" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" s="12">
+        <v>2</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="G46" s="3">
+        <f t="shared" si="2"/>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9">
+      <c r="B47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1.84</v>
+      </c>
+      <c r="G47" s="3">
+        <f t="shared" si="2"/>
+        <v>3.68</v>
+      </c>
+      <c r="I47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9">
+      <c r="B49" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9">
+      <c r="B50" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3">
+        <v>1.62</v>
+      </c>
+      <c r="G50" s="3">
         <f t="shared" si="1"/>
-        <v>0.67</v>
-      </c>
-      <c r="I39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9">
-      <c r="G40" s="3">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9">
+      <c r="B51" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" t="s">
+        <v>72</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="G51" s="3">
+        <f>E51*F51</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9">
+      <c r="B52" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" t="s">
+        <v>74</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" si="1"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9">
+      <c r="B53" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="G53" s="3">
+        <f>E53*F53</f>
+        <v>0</v>
+      </c>
+      <c r="I53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9">
+      <c r="B54" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" t="s">
+        <v>68</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G54" s="3">
+        <f>E54*F54</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9">
+      <c r="B55" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" t="s">
+        <v>69</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="G55" s="3">
+        <f>E55*F55</f>
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9">
+      <c r="B56" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" t="s">
+        <v>67</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="G56" s="3">
+        <f>E56*F56</f>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9">
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="I57" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9">
+      <c r="B60" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" t="s">
+        <v>28</v>
+      </c>
+      <c r="G60" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:9">
-      <c r="B41" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G41" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9">
-      <c r="B42" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" t="s">
-        <v>70</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42" s="3">
-        <v>1.62</v>
-      </c>
-      <c r="G42" s="3">
-        <f t="shared" si="1"/>
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9">
-      <c r="B43" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" t="s">
-        <v>76</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="G43" s="3">
-        <f>E43*F43</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9">
-      <c r="B44" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D44" t="s">
-        <v>78</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-      <c r="F44" s="3">
-        <v>0.36</v>
-      </c>
-      <c r="G44" s="3">
-        <f t="shared" si="1"/>
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9">
-      <c r="B45" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="G45" s="3">
-        <f>E45*F45</f>
-        <v>0</v>
-      </c>
-      <c r="I45" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9">
-      <c r="B46" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" t="s">
-        <v>72</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46" s="3">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G46" s="3">
-        <f>E46*F46</f>
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9">
-      <c r="B47" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47" t="s">
-        <v>73</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47" s="3">
-        <v>0.13</v>
-      </c>
-      <c r="G47" s="3">
-        <f>E47*F47</f>
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9">
-      <c r="B48" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" t="s">
-        <v>71</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-      <c r="F48" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="G48" s="3">
-        <f>E48*F48</f>
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9">
-      <c r="B49" t="s">
-        <v>63</v>
-      </c>
-      <c r="G49" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I49" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9">
-      <c r="G50" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9">
-      <c r="G51" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9">
-      <c r="B52" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" t="s">
-        <v>29</v>
-      </c>
-      <c r="G52" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9">
-      <c r="G58" s="4">
-        <f>SUM(G6:G57)</f>
-        <v>4665.1099999999997</v>
+    <row r="66" spans="7:7">
+      <c r="G66" s="4">
+        <f>SUM(G6:G65)</f>
+        <v>4675.49</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="52" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="48" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>